<commit_message>
Updated My Bench List_15 Apr 20.xlsx
</commit_message>
<xml_diff>
--- a/Bench List_15 Apr 20.xlsx
+++ b/Bench List_15 Apr 20.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bench_status\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3146BE73-9B00-4A3B-A389-88BD86230799}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -19,8 +13,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">List!$A$1:$U$295</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3182" uniqueCount="967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="968">
   <si>
     <t>Country</t>
   </si>
@@ -2925,17 +2919,20 @@
     <t>Not joined status calls</t>
   </si>
   <si>
-    <t>Not joined status call</t>
-  </si>
-  <si>
     <t>Not joines status call</t>
+  </si>
+  <si>
+    <t>From Feb 1st</t>
+  </si>
+  <si>
+    <t>Going through the Training on Java Script and React JS.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2989,6 +2986,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -3069,7 +3073,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3158,11 +3162,14 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 106" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 106" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3432,41 +3439,41 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:W295"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R298" sqref="R298"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A107" sqref="A107:W107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="3" width="8.7265625" style="1"/>
-    <col min="4" max="4" width="23.81640625" style="1" customWidth="1"/>
-    <col min="5" max="7" width="8.7265625" style="1"/>
-    <col min="8" max="8" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7265625" style="1"/>
-    <col min="12" max="12" width="41.54296875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" style="1"/>
-    <col min="14" max="14" width="35.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.7265625" style="1"/>
-    <col min="17" max="17" width="13.54296875" style="1" customWidth="1"/>
-    <col min="18" max="21" width="8.7265625" style="1"/>
-    <col min="22" max="22" width="14.26953125" style="14" customWidth="1"/>
-    <col min="23" max="23" width="21.7265625" style="14" customWidth="1"/>
-    <col min="24" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="3" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="23.85546875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="8.7109375" style="1"/>
+    <col min="8" max="8" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7109375" style="1"/>
+    <col min="12" max="12" width="41.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" style="1"/>
+    <col min="14" max="14" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.7109375" style="1"/>
+    <col min="17" max="17" width="13.5703125" style="1" customWidth="1"/>
+    <col min="18" max="21" width="8.7109375" style="1"/>
+    <col min="22" max="22" width="14.28515625" style="14" customWidth="1"/>
+    <col min="23" max="23" width="21.7109375" style="14" customWidth="1"/>
+    <col min="24" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="33.75">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3537,7 +3544,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" hidden="1">
       <c r="A2" s="8" t="s">
         <v>21</v>
       </c>
@@ -3588,7 +3595,7 @@
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" hidden="1">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -3639,7 +3646,7 @@
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
-    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" hidden="1">
       <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
@@ -3690,7 +3697,7 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
     </row>
-    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" hidden="1">
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
@@ -3741,7 +3748,7 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" hidden="1">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -3792,7 +3799,7 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
     </row>
-    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" hidden="1">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
@@ -3843,7 +3850,7 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
     </row>
-    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" hidden="1">
       <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
@@ -3894,7 +3901,7 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" hidden="1">
       <c r="A9" s="8" t="s">
         <v>21</v>
       </c>
@@ -3945,7 +3952,7 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" hidden="1">
       <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
@@ -3998,7 +4005,7 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" hidden="1">
       <c r="A11" s="8" t="s">
         <v>21</v>
       </c>
@@ -4049,7 +4056,7 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" hidden="1">
       <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
@@ -4100,7 +4107,7 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" hidden="1">
       <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
@@ -4151,7 +4158,7 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" hidden="1">
       <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
@@ -4202,7 +4209,7 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" hidden="1">
       <c r="A15" s="8" t="s">
         <v>21</v>
       </c>
@@ -4253,7 +4260,7 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" hidden="1">
       <c r="A16" s="8" t="s">
         <v>21</v>
       </c>
@@ -4304,7 +4311,7 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
@@ -4353,7 +4360,7 @@
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
     </row>
-    <row r="18" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A18" s="8" t="s">
         <v>21</v>
       </c>
@@ -4402,7 +4409,7 @@
       <c r="T18" s="8"/>
       <c r="U18" s="8"/>
     </row>
-    <row r="19" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A19" s="8" t="s">
         <v>21</v>
       </c>
@@ -4449,7 +4456,7 @@
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
     </row>
-    <row r="20" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A20" s="8" t="s">
         <v>21</v>
       </c>
@@ -4500,7 +4507,7 @@
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
     </row>
-    <row r="21" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A21" s="8" t="s">
         <v>21</v>
       </c>
@@ -4549,7 +4556,7 @@
       <c r="T21" s="8"/>
       <c r="U21" s="8"/>
     </row>
-    <row r="22" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A22" s="8" t="s">
         <v>21</v>
       </c>
@@ -4600,7 +4607,7 @@
       <c r="T22" s="8"/>
       <c r="U22" s="8"/>
     </row>
-    <row r="23" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -4649,7 +4656,7 @@
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
     </row>
-    <row r="24" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A24" s="8" t="s">
         <v>21</v>
       </c>
@@ -4698,7 +4705,7 @@
       <c r="T24" s="8"/>
       <c r="U24" s="8"/>
     </row>
-    <row r="25" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A25" s="8" t="s">
         <v>21</v>
       </c>
@@ -4745,7 +4752,7 @@
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
     </row>
-    <row r="26" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A26" s="8" t="s">
         <v>21</v>
       </c>
@@ -4796,7 +4803,7 @@
       <c r="T26" s="8"/>
       <c r="U26" s="8"/>
     </row>
-    <row r="27" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A27" s="8" t="s">
         <v>21</v>
       </c>
@@ -4847,7 +4854,7 @@
       <c r="T27" s="8"/>
       <c r="U27" s="8"/>
     </row>
-    <row r="28" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A28" s="8" t="s">
         <v>21</v>
       </c>
@@ -4898,7 +4905,7 @@
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
     </row>
-    <row r="29" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A29" s="8" t="s">
         <v>21</v>
       </c>
@@ -4949,7 +4956,7 @@
       <c r="T29" s="8"/>
       <c r="U29" s="8"/>
     </row>
-    <row r="30" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A30" s="8" t="s">
         <v>21</v>
       </c>
@@ -4998,7 +5005,7 @@
       <c r="T30" s="8"/>
       <c r="U30" s="8"/>
     </row>
-    <row r="31" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A31" s="8" t="s">
         <v>21</v>
       </c>
@@ -5047,7 +5054,7 @@
       <c r="T31" s="8"/>
       <c r="U31" s="8"/>
     </row>
-    <row r="32" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A32" s="8" t="s">
         <v>21</v>
       </c>
@@ -5098,7 +5105,7 @@
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
     </row>
-    <row r="33" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A33" s="8" t="s">
         <v>21</v>
       </c>
@@ -5147,7 +5154,7 @@
       <c r="T33" s="8"/>
       <c r="U33" s="8"/>
     </row>
-    <row r="34" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A34" s="8" t="s">
         <v>21</v>
       </c>
@@ -5196,7 +5203,7 @@
       <c r="T34" s="8"/>
       <c r="U34" s="8"/>
     </row>
-    <row r="35" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A35" s="8" t="s">
         <v>21</v>
       </c>
@@ -5245,7 +5252,7 @@
       <c r="T35" s="8"/>
       <c r="U35" s="8"/>
     </row>
-    <row r="36" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A36" s="8" t="s">
         <v>21</v>
       </c>
@@ -5294,7 +5301,7 @@
       <c r="T36" s="8"/>
       <c r="U36" s="8"/>
     </row>
-    <row r="37" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A37" s="8" t="s">
         <v>21</v>
       </c>
@@ -5343,7 +5350,7 @@
       <c r="T37" s="8"/>
       <c r="U37" s="8"/>
     </row>
-    <row r="38" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A38" s="8" t="s">
         <v>21</v>
       </c>
@@ -5392,7 +5399,7 @@
       <c r="T38" s="8"/>
       <c r="U38" s="8"/>
     </row>
-    <row r="39" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A39" s="8" t="s">
         <v>21</v>
       </c>
@@ -5441,7 +5448,7 @@
       <c r="T39" s="8"/>
       <c r="U39" s="8"/>
     </row>
-    <row r="40" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A40" s="8" t="s">
         <v>21</v>
       </c>
@@ -5490,7 +5497,7 @@
       <c r="T40" s="8"/>
       <c r="U40" s="8"/>
     </row>
-    <row r="41" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A41" s="8" t="s">
         <v>21</v>
       </c>
@@ -5539,7 +5546,7 @@
       <c r="T41" s="8"/>
       <c r="U41" s="8"/>
     </row>
-    <row r="42" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A42" s="8" t="s">
         <v>21</v>
       </c>
@@ -5588,7 +5595,7 @@
       <c r="T42" s="8"/>
       <c r="U42" s="8"/>
     </row>
-    <row r="43" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A43" s="8" t="s">
         <v>21</v>
       </c>
@@ -5637,7 +5644,7 @@
       <c r="T43" s="8"/>
       <c r="U43" s="8"/>
     </row>
-    <row r="44" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A44" s="8" t="s">
         <v>21</v>
       </c>
@@ -5686,7 +5693,7 @@
       <c r="T44" s="8"/>
       <c r="U44" s="8"/>
     </row>
-    <row r="45" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A45" s="8" t="s">
         <v>21</v>
       </c>
@@ -5735,7 +5742,7 @@
       <c r="T45" s="8"/>
       <c r="U45" s="8"/>
     </row>
-    <row r="46" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A46" s="8" t="s">
         <v>21</v>
       </c>
@@ -5784,7 +5791,7 @@
       <c r="T46" s="8"/>
       <c r="U46" s="8"/>
     </row>
-    <row r="47" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A47" s="8" t="s">
         <v>21</v>
       </c>
@@ -5833,7 +5840,7 @@
       <c r="T47" s="8"/>
       <c r="U47" s="8"/>
     </row>
-    <row r="48" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A48" s="8" t="s">
         <v>21</v>
       </c>
@@ -5884,7 +5891,7 @@
       <c r="T48" s="8"/>
       <c r="U48" s="8"/>
     </row>
-    <row r="49" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" hidden="1">
       <c r="A49" s="8" t="s">
         <v>21</v>
       </c>
@@ -5935,7 +5942,7 @@
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
     </row>
-    <row r="50" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" hidden="1">
       <c r="A50" s="8" t="s">
         <v>21</v>
       </c>
@@ -5984,7 +5991,7 @@
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
     </row>
-    <row r="51" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" hidden="1">
       <c r="A51" s="8" t="s">
         <v>21</v>
       </c>
@@ -6033,7 +6040,7 @@
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
     </row>
-    <row r="52" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" hidden="1">
       <c r="A52" s="8" t="s">
         <v>21</v>
       </c>
@@ -6084,7 +6091,7 @@
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
     </row>
-    <row r="53" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" hidden="1">
       <c r="A53" s="8" t="s">
         <v>21</v>
       </c>
@@ -6135,7 +6142,7 @@
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
     </row>
-    <row r="54" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" hidden="1">
       <c r="A54" s="8" t="s">
         <v>21</v>
       </c>
@@ -6188,7 +6195,7 @@
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
     </row>
-    <row r="55" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" hidden="1">
       <c r="A55" s="8" t="s">
         <v>21</v>
       </c>
@@ -6239,7 +6246,7 @@
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
     </row>
-    <row r="56" spans="1:23" ht="32.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" ht="45.75">
       <c r="A56" s="8" t="s">
         <v>21</v>
       </c>
@@ -6304,7 +6311,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="57" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" hidden="1">
       <c r="A57" s="8" t="s">
         <v>21</v>
       </c>
@@ -6355,7 +6362,7 @@
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
     </row>
-    <row r="58" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" hidden="1">
       <c r="A58" s="8" t="s">
         <v>21</v>
       </c>
@@ -6404,7 +6411,7 @@
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
     </row>
-    <row r="59" spans="1:23" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" s="19" customFormat="1" ht="16.5" customHeight="1">
       <c r="A59" s="22" t="s">
         <v>21</v>
       </c>
@@ -6463,11 +6470,11 @@
       <c r="T59" s="22"/>
       <c r="U59" s="22"/>
       <c r="V59" s="22" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="W59" s="27"/>
     </row>
-    <row r="60" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" hidden="1">
       <c r="A60" s="8" t="s">
         <v>21</v>
       </c>
@@ -6518,7 +6525,7 @@
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
     </row>
-    <row r="61" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" hidden="1">
       <c r="A61" s="8" t="s">
         <v>21</v>
       </c>
@@ -6569,7 +6576,7 @@
       <c r="V61" s="1"/>
       <c r="W61" s="1"/>
     </row>
-    <row r="62" spans="1:23" ht="22" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" ht="23.25">
       <c r="A62" s="8" t="s">
         <v>21</v>
       </c>
@@ -6634,7 +6641,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="63" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" hidden="1">
       <c r="A63" s="8" t="s">
         <v>21</v>
       </c>
@@ -6685,7 +6692,7 @@
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
     </row>
-    <row r="64" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:23" ht="15.75" customHeight="1">
       <c r="A64" s="8" t="s">
         <v>21</v>
       </c>
@@ -6750,7 +6757,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="65" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" hidden="1">
       <c r="A65" s="8" t="s">
         <v>21</v>
       </c>
@@ -6801,7 +6808,7 @@
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
     </row>
-    <row r="66" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" ht="33.75">
       <c r="A66" s="8" t="s">
         <v>21</v>
       </c>
@@ -6866,7 +6873,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="67" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" hidden="1">
       <c r="A67" s="8" t="s">
         <v>21</v>
       </c>
@@ -6917,7 +6924,7 @@
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
     </row>
-    <row r="68" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" hidden="1">
       <c r="A68" s="8" t="s">
         <v>21</v>
       </c>
@@ -6970,7 +6977,7 @@
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
     </row>
-    <row r="69" spans="1:23" s="19" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" s="19" customFormat="1" ht="22.5">
       <c r="A69" s="15" t="s">
         <v>21</v>
       </c>
@@ -7035,7 +7042,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="70" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" hidden="1">
       <c r="A70" s="8" t="s">
         <v>21</v>
       </c>
@@ -7086,7 +7093,7 @@
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
     </row>
-    <row r="71" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" hidden="1">
       <c r="A71" s="8" t="s">
         <v>21</v>
       </c>
@@ -7137,7 +7144,7 @@
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
     </row>
-    <row r="72" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" hidden="1">
       <c r="A72" s="8" t="s">
         <v>21</v>
       </c>
@@ -7188,7 +7195,7 @@
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
     </row>
-    <row r="73" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" hidden="1">
       <c r="A73" s="8" t="s">
         <v>21</v>
       </c>
@@ -7239,7 +7246,7 @@
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
     </row>
-    <row r="74" spans="1:23" s="19" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" s="19" customFormat="1" ht="15">
       <c r="A74" s="15" t="s">
         <v>21</v>
       </c>
@@ -7300,7 +7307,7 @@
       <c r="V74" s="21"/>
       <c r="W74" s="21"/>
     </row>
-    <row r="75" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" hidden="1">
       <c r="A75" s="8" t="s">
         <v>21</v>
       </c>
@@ -7351,7 +7358,7 @@
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
     </row>
-    <row r="76" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" hidden="1">
       <c r="A76" s="8" t="s">
         <v>21</v>
       </c>
@@ -7404,7 +7411,7 @@
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
     </row>
-    <row r="77" spans="1:23" ht="22" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:23" ht="23.25">
       <c r="A77" s="8" t="s">
         <v>21</v>
       </c>
@@ -7469,7 +7476,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="78" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" hidden="1">
       <c r="A78" s="8" t="s">
         <v>21</v>
       </c>
@@ -7520,7 +7527,7 @@
       <c r="V78" s="1"/>
       <c r="W78" s="1"/>
     </row>
-    <row r="79" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" hidden="1">
       <c r="A79" s="8" t="s">
         <v>21</v>
       </c>
@@ -7571,7 +7578,7 @@
       <c r="V79" s="1"/>
       <c r="W79" s="1"/>
     </row>
-    <row r="80" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" hidden="1">
       <c r="A80" s="8" t="s">
         <v>21</v>
       </c>
@@ -7624,7 +7631,7 @@
       <c r="V80" s="1"/>
       <c r="W80" s="1"/>
     </row>
-    <row r="81" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" ht="33.75">
       <c r="A81" s="8" t="s">
         <v>21</v>
       </c>
@@ -7689,7 +7696,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="82" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" hidden="1">
       <c r="A82" s="8" t="s">
         <v>21</v>
       </c>
@@ -7742,7 +7749,7 @@
       <c r="V82" s="1"/>
       <c r="W82" s="1"/>
     </row>
-    <row r="83" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" hidden="1">
       <c r="A83" s="8" t="s">
         <v>21</v>
       </c>
@@ -7793,7 +7800,7 @@
       <c r="V83" s="1"/>
       <c r="W83" s="1"/>
     </row>
-    <row r="84" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" hidden="1">
       <c r="A84" s="8" t="s">
         <v>21</v>
       </c>
@@ -7844,7 +7851,7 @@
       <c r="V84" s="1"/>
       <c r="W84" s="1"/>
     </row>
-    <row r="85" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" hidden="1">
       <c r="A85" s="8" t="s">
         <v>21</v>
       </c>
@@ -7897,7 +7904,7 @@
       <c r="V85" s="1"/>
       <c r="W85" s="1"/>
     </row>
-    <row r="86" spans="1:23" s="19" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:23" s="19" customFormat="1" ht="15">
       <c r="A86" s="15" t="s">
         <v>21</v>
       </c>
@@ -7958,7 +7965,7 @@
       <c r="V86" s="21"/>
       <c r="W86" s="21"/>
     </row>
-    <row r="87" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" hidden="1">
       <c r="A87" s="8" t="s">
         <v>21</v>
       </c>
@@ -8009,7 +8016,7 @@
       <c r="V87" s="1"/>
       <c r="W87" s="1"/>
     </row>
-    <row r="88" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" hidden="1">
       <c r="A88" s="8" t="s">
         <v>21</v>
       </c>
@@ -8060,7 +8067,7 @@
       <c r="V88" s="1"/>
       <c r="W88" s="1"/>
     </row>
-    <row r="89" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" hidden="1">
       <c r="A89" s="8" t="s">
         <v>21</v>
       </c>
@@ -8111,7 +8118,7 @@
       <c r="V89" s="1"/>
       <c r="W89" s="1"/>
     </row>
-    <row r="90" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" ht="33.75">
       <c r="A90" s="8" t="s">
         <v>21</v>
       </c>
@@ -8176,7 +8183,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="91" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" hidden="1">
       <c r="A91" s="8" t="s">
         <v>21</v>
       </c>
@@ -8229,7 +8236,7 @@
       <c r="V91" s="1"/>
       <c r="W91" s="1"/>
     </row>
-    <row r="92" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" hidden="1">
       <c r="A92" s="8" t="s">
         <v>21</v>
       </c>
@@ -8280,7 +8287,7 @@
       <c r="V92" s="1"/>
       <c r="W92" s="1"/>
     </row>
-    <row r="93" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" hidden="1">
       <c r="A93" s="8" t="s">
         <v>21</v>
       </c>
@@ -8331,7 +8338,7 @@
       <c r="V93" s="1"/>
       <c r="W93" s="1"/>
     </row>
-    <row r="94" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" hidden="1">
       <c r="A94" s="8" t="s">
         <v>21</v>
       </c>
@@ -8384,7 +8391,7 @@
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
     </row>
-    <row r="95" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" hidden="1">
       <c r="A95" s="8" t="s">
         <v>21</v>
       </c>
@@ -8437,7 +8444,7 @@
       <c r="V95" s="1"/>
       <c r="W95" s="1"/>
     </row>
-    <row r="96" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" hidden="1">
       <c r="A96" s="8" t="s">
         <v>21</v>
       </c>
@@ -8488,7 +8495,7 @@
       <c r="V96" s="1"/>
       <c r="W96" s="1"/>
     </row>
-    <row r="97" spans="1:23" s="19" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:23" s="19" customFormat="1" ht="15">
       <c r="A97" s="28" t="s">
         <v>21</v>
       </c>
@@ -8545,7 +8552,7 @@
       <c r="V97" s="33"/>
       <c r="W97" s="33"/>
     </row>
-    <row r="98" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" hidden="1">
       <c r="A98" s="8" t="s">
         <v>21</v>
       </c>
@@ -8596,7 +8603,7 @@
       <c r="V98" s="1"/>
       <c r="W98" s="1"/>
     </row>
-    <row r="99" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" hidden="1">
       <c r="A99" s="8" t="s">
         <v>21</v>
       </c>
@@ -8647,7 +8654,7 @@
       <c r="V99" s="1"/>
       <c r="W99" s="1"/>
     </row>
-    <row r="100" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" hidden="1">
       <c r="A100" s="8" t="s">
         <v>21</v>
       </c>
@@ -8698,7 +8705,7 @@
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
     </row>
-    <row r="101" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" hidden="1">
       <c r="A101" s="8" t="s">
         <v>21</v>
       </c>
@@ -8749,7 +8756,7 @@
       <c r="V101" s="1"/>
       <c r="W101" s="1"/>
     </row>
-    <row r="102" spans="1:23" s="19" customFormat="1" ht="22" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:23" s="19" customFormat="1" ht="23.25">
       <c r="A102" s="15" t="s">
         <v>21</v>
       </c>
@@ -8814,7 +8821,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="103" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" hidden="1">
       <c r="A103" s="8" t="s">
         <v>21</v>
       </c>
@@ -8867,7 +8874,7 @@
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
     </row>
-    <row r="104" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" hidden="1">
       <c r="A104" s="8" t="s">
         <v>21</v>
       </c>
@@ -8918,7 +8925,7 @@
       <c r="V104" s="1"/>
       <c r="W104" s="1"/>
     </row>
-    <row r="105" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" hidden="1">
       <c r="A105" s="8" t="s">
         <v>21</v>
       </c>
@@ -8969,7 +8976,7 @@
       <c r="V105" s="1"/>
       <c r="W105" s="1"/>
     </row>
-    <row r="106" spans="1:23" s="19" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" s="19" customFormat="1" ht="22.5">
       <c r="A106" s="15" t="s">
         <v>21</v>
       </c>
@@ -9034,70 +9041,72 @@
         <v>956</v>
       </c>
     </row>
-    <row r="107" spans="1:23" s="19" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B107" s="23">
+    <row r="107" spans="1:23" s="19" customFormat="1" ht="23.25">
+      <c r="A107" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B107" s="10">
         <v>1285150</v>
       </c>
-      <c r="C107" s="23">
+      <c r="C107" s="10">
         <v>142584</v>
       </c>
-      <c r="D107" s="23" t="s">
+      <c r="D107" s="10" t="s">
         <v>373</v>
       </c>
-      <c r="E107" s="23" t="s">
+      <c r="E107" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F107" s="22" t="s">
+      <c r="F107" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="G107" s="22" t="s">
+      <c r="G107" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="H107" s="24">
+      <c r="H107" s="16">
         <v>43082</v>
       </c>
-      <c r="I107" s="25" t="s">
+      <c r="I107" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="J107" s="25" t="s">
+      <c r="J107" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K107" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="L107" s="26" t="s">
+      <c r="K107" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L107" s="34" t="s">
         <v>374</v>
       </c>
-      <c r="M107" s="23" t="s">
+      <c r="M107" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="N107" s="22" t="s">
+      <c r="N107" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="O107" s="22" t="s">
+      <c r="O107" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="P107" s="22" t="s">
+      <c r="P107" s="15" t="s">
         <v>936</v>
       </c>
-      <c r="Q107" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="R107" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="S107" s="22"/>
-      <c r="T107" s="22"/>
-      <c r="U107" s="22"/>
-      <c r="V107" s="27" t="s">
-        <v>965</v>
-      </c>
-      <c r="W107" s="27"/>
-    </row>
-    <row r="108" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+      <c r="Q107" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="R107" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="S107" s="15"/>
+      <c r="T107" s="15"/>
+      <c r="U107" s="15"/>
+      <c r="V107" s="21" t="s">
+        <v>966</v>
+      </c>
+      <c r="W107" s="21" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" hidden="1">
       <c r="A108" s="8" t="s">
         <v>21</v>
       </c>
@@ -9150,7 +9159,7 @@
       <c r="V108" s="1"/>
       <c r="W108" s="1"/>
     </row>
-    <row r="109" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" hidden="1">
       <c r="A109" s="8" t="s">
         <v>21</v>
       </c>
@@ -9201,7 +9210,7 @@
       <c r="V109" s="1"/>
       <c r="W109" s="1"/>
     </row>
-    <row r="110" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" hidden="1">
       <c r="A110" s="8" t="s">
         <v>21</v>
       </c>
@@ -9254,7 +9263,7 @@
       <c r="V110" s="1"/>
       <c r="W110" s="1"/>
     </row>
-    <row r="111" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" hidden="1">
       <c r="A111" s="8" t="s">
         <v>21</v>
       </c>
@@ -9305,7 +9314,7 @@
       <c r="V111" s="1"/>
       <c r="W111" s="1"/>
     </row>
-    <row r="112" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" hidden="1">
       <c r="A112" s="8" t="s">
         <v>21</v>
       </c>
@@ -9356,7 +9365,7 @@
       <c r="V112" s="1"/>
       <c r="W112" s="1"/>
     </row>
-    <row r="113" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" hidden="1">
       <c r="A113" s="8" t="s">
         <v>21</v>
       </c>
@@ -9409,7 +9418,7 @@
       <c r="V113" s="1"/>
       <c r="W113" s="1"/>
     </row>
-    <row r="114" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:23" hidden="1">
       <c r="A114" s="8" t="s">
         <v>21</v>
       </c>
@@ -9460,7 +9469,7 @@
       <c r="V114" s="1"/>
       <c r="W114" s="1"/>
     </row>
-    <row r="115" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:23" hidden="1">
       <c r="A115" s="8" t="s">
         <v>21</v>
       </c>
@@ -9511,7 +9520,7 @@
       <c r="V115" s="1"/>
       <c r="W115" s="1"/>
     </row>
-    <row r="116" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" hidden="1">
       <c r="A116" s="8" t="s">
         <v>21</v>
       </c>
@@ -9562,7 +9571,7 @@
       <c r="V116" s="1"/>
       <c r="W116" s="1"/>
     </row>
-    <row r="117" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" hidden="1">
       <c r="A117" s="8" t="s">
         <v>21</v>
       </c>
@@ -9615,7 +9624,7 @@
       <c r="V117" s="1"/>
       <c r="W117" s="1"/>
     </row>
-    <row r="118" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:23" hidden="1">
       <c r="A118" s="8" t="s">
         <v>21</v>
       </c>
@@ -9668,7 +9677,7 @@
       <c r="V118" s="1"/>
       <c r="W118" s="1"/>
     </row>
-    <row r="119" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" hidden="1">
       <c r="A119" s="8" t="s">
         <v>21</v>
       </c>
@@ -9721,7 +9730,7 @@
       <c r="V119" s="1"/>
       <c r="W119" s="1"/>
     </row>
-    <row r="120" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" hidden="1">
       <c r="A120" s="8" t="s">
         <v>21</v>
       </c>
@@ -9772,7 +9781,7 @@
       <c r="V120" s="1"/>
       <c r="W120" s="1"/>
     </row>
-    <row r="121" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" hidden="1">
       <c r="A121" s="8" t="s">
         <v>21</v>
       </c>
@@ -9825,7 +9834,7 @@
       <c r="V121" s="1"/>
       <c r="W121" s="1"/>
     </row>
-    <row r="122" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" hidden="1">
       <c r="A122" s="8" t="s">
         <v>21</v>
       </c>
@@ -9876,7 +9885,7 @@
       <c r="V122" s="1"/>
       <c r="W122" s="1"/>
     </row>
-    <row r="123" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" hidden="1">
       <c r="A123" s="8" t="s">
         <v>21</v>
       </c>
@@ -9927,7 +9936,7 @@
       <c r="V123" s="1"/>
       <c r="W123" s="1"/>
     </row>
-    <row r="124" spans="1:23" s="19" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:23" s="19" customFormat="1" ht="23.25">
       <c r="A124" s="22" t="s">
         <v>21</v>
       </c>
@@ -9986,11 +9995,11 @@
       <c r="T124" s="22"/>
       <c r="U124" s="22"/>
       <c r="V124" s="27" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="W124" s="27"/>
     </row>
-    <row r="125" spans="1:23" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:23" ht="23.25">
       <c r="A125" s="8" t="s">
         <v>21</v>
       </c>
@@ -10055,7 +10064,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="126" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" hidden="1">
       <c r="A126" s="8" t="s">
         <v>21</v>
       </c>
@@ -10106,7 +10115,7 @@
       <c r="V126" s="1"/>
       <c r="W126" s="1"/>
     </row>
-    <row r="127" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" ht="22.5">
       <c r="A127" s="8" t="s">
         <v>21</v>
       </c>
@@ -10171,7 +10180,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="128" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" hidden="1">
       <c r="A128" s="8" t="s">
         <v>21</v>
       </c>
@@ -10222,7 +10231,7 @@
       <c r="V128" s="1"/>
       <c r="W128" s="1"/>
     </row>
-    <row r="129" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" hidden="1">
       <c r="A129" s="8" t="s">
         <v>21</v>
       </c>
@@ -10273,7 +10282,7 @@
       <c r="V129" s="1"/>
       <c r="W129" s="1"/>
     </row>
-    <row r="130" spans="1:23" s="19" customFormat="1" ht="22" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:23" s="19" customFormat="1" ht="34.5">
       <c r="A130" s="15" t="s">
         <v>21</v>
       </c>
@@ -10338,7 +10347,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="131" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23" hidden="1">
       <c r="A131" s="8" t="s">
         <v>21</v>
       </c>
@@ -10391,7 +10400,7 @@
       <c r="V131" s="1"/>
       <c r="W131" s="1"/>
     </row>
-    <row r="132" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:23" hidden="1">
       <c r="A132" s="8" t="s">
         <v>21</v>
       </c>
@@ -10444,7 +10453,7 @@
       <c r="V132" s="1"/>
       <c r="W132" s="1"/>
     </row>
-    <row r="133" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:23" hidden="1">
       <c r="A133" s="8" t="s">
         <v>21</v>
       </c>
@@ -10495,7 +10504,7 @@
       <c r="V133" s="1"/>
       <c r="W133" s="1"/>
     </row>
-    <row r="134" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23" hidden="1">
       <c r="A134" s="8" t="s">
         <v>21</v>
       </c>
@@ -10546,7 +10555,7 @@
       <c r="V134" s="1"/>
       <c r="W134" s="1"/>
     </row>
-    <row r="135" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23" hidden="1">
       <c r="A135" s="8" t="s">
         <v>21</v>
       </c>
@@ -10599,7 +10608,7 @@
       <c r="V135" s="1"/>
       <c r="W135" s="1"/>
     </row>
-    <row r="136" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" hidden="1">
       <c r="A136" s="8" t="s">
         <v>21</v>
       </c>
@@ -10650,7 +10659,7 @@
       <c r="V136" s="1"/>
       <c r="W136" s="1"/>
     </row>
-    <row r="137" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:23" hidden="1">
       <c r="A137" s="8" t="s">
         <v>21</v>
       </c>
@@ -10701,7 +10710,7 @@
       <c r="V137" s="1"/>
       <c r="W137" s="1"/>
     </row>
-    <row r="138" spans="1:23" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:23" s="19" customFormat="1">
       <c r="A138" s="15" t="s">
         <v>21</v>
       </c>
@@ -10762,7 +10771,7 @@
       <c r="V138" s="21"/>
       <c r="W138" s="21"/>
     </row>
-    <row r="139" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:23" hidden="1">
       <c r="A139" s="8" t="s">
         <v>21</v>
       </c>
@@ -10815,7 +10824,7 @@
       <c r="V139" s="1"/>
       <c r="W139" s="1"/>
     </row>
-    <row r="140" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23" hidden="1">
       <c r="A140" s="8" t="s">
         <v>21</v>
       </c>
@@ -10868,7 +10877,7 @@
       <c r="V140" s="1"/>
       <c r="W140" s="1"/>
     </row>
-    <row r="141" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23" hidden="1">
       <c r="A141" s="8" t="s">
         <v>21</v>
       </c>
@@ -10921,7 +10930,7 @@
       <c r="V141" s="1"/>
       <c r="W141" s="1"/>
     </row>
-    <row r="142" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23" hidden="1">
       <c r="A142" s="8" t="s">
         <v>21</v>
       </c>
@@ -10972,7 +10981,7 @@
       <c r="V142" s="1"/>
       <c r="W142" s="1"/>
     </row>
-    <row r="143" spans="1:23" ht="22" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:23" ht="23.25">
       <c r="A143" s="8" t="s">
         <v>21</v>
       </c>
@@ -11037,7 +11046,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="144" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:23" hidden="1">
       <c r="A144" s="8" t="s">
         <v>21</v>
       </c>
@@ -11088,7 +11097,7 @@
       <c r="V144" s="1"/>
       <c r="W144" s="1"/>
     </row>
-    <row r="145" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:23" hidden="1">
       <c r="A145" s="8" t="s">
         <v>21</v>
       </c>
@@ -11141,7 +11150,7 @@
       <c r="V145" s="1"/>
       <c r="W145" s="1"/>
     </row>
-    <row r="146" spans="1:23" s="19" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:23" s="19" customFormat="1" ht="23.25">
       <c r="A146" s="22" t="s">
         <v>21</v>
       </c>
@@ -11204,7 +11213,7 @@
       </c>
       <c r="W146" s="27"/>
     </row>
-    <row r="147" spans="1:23" s="19" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:23" s="19" customFormat="1" ht="23.25">
       <c r="A147" s="22" t="s">
         <v>21</v>
       </c>
@@ -11267,7 +11276,7 @@
       </c>
       <c r="W147" s="27"/>
     </row>
-    <row r="148" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:23" hidden="1">
       <c r="A148" s="8" t="s">
         <v>21</v>
       </c>
@@ -11318,7 +11327,7 @@
       <c r="V148" s="1"/>
       <c r="W148" s="1"/>
     </row>
-    <row r="149" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:23" hidden="1">
       <c r="A149" s="8" t="s">
         <v>21</v>
       </c>
@@ -11371,7 +11380,7 @@
       <c r="V149" s="1"/>
       <c r="W149" s="1"/>
     </row>
-    <row r="150" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:23" hidden="1">
       <c r="A150" s="8" t="s">
         <v>21</v>
       </c>
@@ -11424,7 +11433,7 @@
       <c r="V150" s="1"/>
       <c r="W150" s="1"/>
     </row>
-    <row r="151" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:23" hidden="1">
       <c r="A151" s="8" t="s">
         <v>21</v>
       </c>
@@ -11473,7 +11482,7 @@
       <c r="V151" s="1"/>
       <c r="W151" s="1"/>
     </row>
-    <row r="152" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:23" hidden="1">
       <c r="A152" s="8" t="s">
         <v>21</v>
       </c>
@@ -11524,7 +11533,7 @@
       <c r="V152" s="1"/>
       <c r="W152" s="1"/>
     </row>
-    <row r="153" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:23" hidden="1">
       <c r="A153" s="8" t="s">
         <v>21</v>
       </c>
@@ -11575,7 +11584,7 @@
       <c r="V153" s="1"/>
       <c r="W153" s="1"/>
     </row>
-    <row r="154" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:23" hidden="1">
       <c r="A154" s="8" t="s">
         <v>21</v>
       </c>
@@ -11628,7 +11637,7 @@
       <c r="V154" s="1"/>
       <c r="W154" s="1"/>
     </row>
-    <row r="155" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:23" hidden="1">
       <c r="A155" s="8" t="s">
         <v>21</v>
       </c>
@@ -11679,7 +11688,7 @@
       <c r="V155" s="1"/>
       <c r="W155" s="1"/>
     </row>
-    <row r="156" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:23" hidden="1">
       <c r="A156" s="8" t="s">
         <v>21</v>
       </c>
@@ -11730,7 +11739,7 @@
       <c r="V156" s="1"/>
       <c r="W156" s="1"/>
     </row>
-    <row r="157" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:23" hidden="1">
       <c r="A157" s="8" t="s">
         <v>21</v>
       </c>
@@ -11781,7 +11790,7 @@
       <c r="V157" s="1"/>
       <c r="W157" s="1"/>
     </row>
-    <row r="158" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:23" hidden="1">
       <c r="A158" s="8" t="s">
         <v>21</v>
       </c>
@@ -11832,7 +11841,7 @@
       <c r="V158" s="1"/>
       <c r="W158" s="1"/>
     </row>
-    <row r="159" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:23" hidden="1">
       <c r="A159" s="8" t="s">
         <v>21</v>
       </c>
@@ -11885,7 +11894,7 @@
       <c r="V159" s="1"/>
       <c r="W159" s="1"/>
     </row>
-    <row r="160" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:23" hidden="1">
       <c r="A160" s="8" t="s">
         <v>21</v>
       </c>
@@ -11936,7 +11945,7 @@
       <c r="V160" s="1"/>
       <c r="W160" s="1"/>
     </row>
-    <row r="161" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A161" s="8" t="s">
         <v>21</v>
       </c>
@@ -11985,7 +11994,7 @@
       <c r="T161" s="8"/>
       <c r="U161" s="8"/>
     </row>
-    <row r="162" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A162" s="8" t="s">
         <v>21</v>
       </c>
@@ -12034,7 +12043,7 @@
       <c r="T162" s="8"/>
       <c r="U162" s="8"/>
     </row>
-    <row r="163" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A163" s="8" t="s">
         <v>21</v>
       </c>
@@ -12083,7 +12092,7 @@
       <c r="T163" s="8"/>
       <c r="U163" s="8"/>
     </row>
-    <row r="164" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A164" s="8" t="s">
         <v>21</v>
       </c>
@@ -12134,7 +12143,7 @@
       <c r="T164" s="8"/>
       <c r="U164" s="8"/>
     </row>
-    <row r="165" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A165" s="8" t="s">
         <v>21</v>
       </c>
@@ -12183,7 +12192,7 @@
       <c r="T165" s="8"/>
       <c r="U165" s="8"/>
     </row>
-    <row r="166" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A166" s="8" t="s">
         <v>21</v>
       </c>
@@ -12232,7 +12241,7 @@
       <c r="T166" s="8"/>
       <c r="U166" s="8"/>
     </row>
-    <row r="167" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A167" s="8" t="s">
         <v>21</v>
       </c>
@@ -12281,7 +12290,7 @@
       <c r="T167" s="8"/>
       <c r="U167" s="8"/>
     </row>
-    <row r="168" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A168" s="8" t="s">
         <v>21</v>
       </c>
@@ -12330,7 +12339,7 @@
       <c r="T168" s="8"/>
       <c r="U168" s="8"/>
     </row>
-    <row r="169" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A169" s="8" t="s">
         <v>21</v>
       </c>
@@ -12379,7 +12388,7 @@
       <c r="T169" s="8"/>
       <c r="U169" s="8"/>
     </row>
-    <row r="170" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A170" s="8" t="s">
         <v>21</v>
       </c>
@@ -12428,7 +12437,7 @@
       <c r="T170" s="8"/>
       <c r="U170" s="8"/>
     </row>
-    <row r="171" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A171" s="8" t="s">
         <v>21</v>
       </c>
@@ -12477,7 +12486,7 @@
       <c r="T171" s="8"/>
       <c r="U171" s="8"/>
     </row>
-    <row r="172" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A172" s="8" t="s">
         <v>21</v>
       </c>
@@ -12526,7 +12535,7 @@
       <c r="T172" s="8"/>
       <c r="U172" s="8"/>
     </row>
-    <row r="173" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A173" s="8" t="s">
         <v>21</v>
       </c>
@@ -12575,7 +12584,7 @@
       <c r="T173" s="8"/>
       <c r="U173" s="8"/>
     </row>
-    <row r="174" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A174" s="8" t="s">
         <v>21</v>
       </c>
@@ -12624,7 +12633,7 @@
       <c r="T174" s="8"/>
       <c r="U174" s="8"/>
     </row>
-    <row r="175" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A175" s="8" t="s">
         <v>21</v>
       </c>
@@ -12673,7 +12682,7 @@
       <c r="T175" s="8"/>
       <c r="U175" s="8"/>
     </row>
-    <row r="176" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A176" s="8" t="s">
         <v>21</v>
       </c>
@@ -12722,7 +12731,7 @@
       <c r="T176" s="8"/>
       <c r="U176" s="8"/>
     </row>
-    <row r="177" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A177" s="8" t="s">
         <v>21</v>
       </c>
@@ -12771,7 +12780,7 @@
       <c r="T177" s="8"/>
       <c r="U177" s="8"/>
     </row>
-    <row r="178" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A178" s="8" t="s">
         <v>21</v>
       </c>
@@ -12822,7 +12831,7 @@
       <c r="T178" s="8"/>
       <c r="U178" s="8"/>
     </row>
-    <row r="179" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A179" s="8" t="s">
         <v>21</v>
       </c>
@@ -12871,7 +12880,7 @@
       <c r="T179" s="8"/>
       <c r="U179" s="8"/>
     </row>
-    <row r="180" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A180" s="8" t="s">
         <v>21</v>
       </c>
@@ -12922,7 +12931,7 @@
       <c r="T180" s="8"/>
       <c r="U180" s="8"/>
     </row>
-    <row r="181" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A181" s="8" t="s">
         <v>21</v>
       </c>
@@ -12973,7 +12982,7 @@
       <c r="T181" s="8"/>
       <c r="U181" s="8"/>
     </row>
-    <row r="182" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A182" s="8" t="s">
         <v>21</v>
       </c>
@@ -13022,7 +13031,7 @@
       <c r="T182" s="8"/>
       <c r="U182" s="8"/>
     </row>
-    <row r="183" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A183" s="8" t="s">
         <v>21</v>
       </c>
@@ -13071,7 +13080,7 @@
       <c r="T183" s="8"/>
       <c r="U183" s="8"/>
     </row>
-    <row r="184" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A184" s="8" t="s">
         <v>21</v>
       </c>
@@ -13120,7 +13129,7 @@
       <c r="T184" s="8"/>
       <c r="U184" s="8"/>
     </row>
-    <row r="185" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A185" s="8" t="s">
         <v>21</v>
       </c>
@@ -13171,7 +13180,7 @@
       <c r="T185" s="8"/>
       <c r="U185" s="8"/>
     </row>
-    <row r="186" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A186" s="8" t="s">
         <v>21</v>
       </c>
@@ -13220,7 +13229,7 @@
       <c r="T186" s="8"/>
       <c r="U186" s="8"/>
     </row>
-    <row r="187" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A187" s="8" t="s">
         <v>21</v>
       </c>
@@ -13271,7 +13280,7 @@
       <c r="T187" s="8"/>
       <c r="U187" s="8"/>
     </row>
-    <row r="188" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A188" s="8" t="s">
         <v>21</v>
       </c>
@@ -13320,7 +13329,7 @@
       <c r="T188" s="8"/>
       <c r="U188" s="8"/>
     </row>
-    <row r="189" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A189" s="8" t="s">
         <v>21</v>
       </c>
@@ -13369,7 +13378,7 @@
       <c r="T189" s="8"/>
       <c r="U189" s="8"/>
     </row>
-    <row r="190" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A190" s="8" t="s">
         <v>21</v>
       </c>
@@ -13418,7 +13427,7 @@
       <c r="T190" s="8"/>
       <c r="U190" s="8"/>
     </row>
-    <row r="191" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A191" s="8" t="s">
         <v>21</v>
       </c>
@@ -13465,7 +13474,7 @@
       <c r="T191" s="8"/>
       <c r="U191" s="8"/>
     </row>
-    <row r="192" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A192" s="8" t="s">
         <v>21</v>
       </c>
@@ -13514,7 +13523,7 @@
       <c r="T192" s="8"/>
       <c r="U192" s="8"/>
     </row>
-    <row r="193" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A193" s="8" t="s">
         <v>21</v>
       </c>
@@ -13565,7 +13574,7 @@
       <c r="T193" s="8"/>
       <c r="U193" s="8"/>
     </row>
-    <row r="194" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A194" s="8" t="s">
         <v>21</v>
       </c>
@@ -13616,7 +13625,7 @@
       <c r="T194" s="8"/>
       <c r="U194" s="8"/>
     </row>
-    <row r="195" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A195" s="8" t="s">
         <v>21</v>
       </c>
@@ -13665,7 +13674,7 @@
       <c r="T195" s="8"/>
       <c r="U195" s="8"/>
     </row>
-    <row r="196" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A196" s="8" t="s">
         <v>21</v>
       </c>
@@ -13716,7 +13725,7 @@
       <c r="T196" s="8"/>
       <c r="U196" s="8"/>
     </row>
-    <row r="197" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A197" s="8" t="s">
         <v>21</v>
       </c>
@@ -13765,7 +13774,7 @@
       <c r="T197" s="8"/>
       <c r="U197" s="8"/>
     </row>
-    <row r="198" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A198" s="8" t="s">
         <v>21</v>
       </c>
@@ -13814,7 +13823,7 @@
       <c r="T198" s="8"/>
       <c r="U198" s="8"/>
     </row>
-    <row r="199" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A199" s="8" t="s">
         <v>21</v>
       </c>
@@ -13863,7 +13872,7 @@
       <c r="T199" s="8"/>
       <c r="U199" s="8"/>
     </row>
-    <row r="200" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A200" s="8" t="s">
         <v>21</v>
       </c>
@@ -13912,7 +13921,7 @@
       <c r="T200" s="8"/>
       <c r="U200" s="8"/>
     </row>
-    <row r="201" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A201" s="8" t="s">
         <v>21</v>
       </c>
@@ -13961,7 +13970,7 @@
       <c r="T201" s="8"/>
       <c r="U201" s="8"/>
     </row>
-    <row r="202" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A202" s="8" t="s">
         <v>21</v>
       </c>
@@ -14008,7 +14017,7 @@
       <c r="T202" s="8"/>
       <c r="U202" s="8"/>
     </row>
-    <row r="203" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A203" s="8" t="s">
         <v>21</v>
       </c>
@@ -14057,7 +14066,7 @@
       <c r="T203" s="8"/>
       <c r="U203" s="8"/>
     </row>
-    <row r="204" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A204" s="8" t="s">
         <v>21</v>
       </c>
@@ -14106,7 +14115,7 @@
       <c r="T204" s="8"/>
       <c r="U204" s="8"/>
     </row>
-    <row r="205" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A205" s="8" t="s">
         <v>21</v>
       </c>
@@ -14155,7 +14164,7 @@
       <c r="T205" s="8"/>
       <c r="U205" s="8"/>
     </row>
-    <row r="206" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A206" s="8" t="s">
         <v>21</v>
       </c>
@@ -14204,7 +14213,7 @@
       <c r="T206" s="8"/>
       <c r="U206" s="8"/>
     </row>
-    <row r="207" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A207" s="8" t="s">
         <v>21</v>
       </c>
@@ -14253,7 +14262,7 @@
       <c r="T207" s="8"/>
       <c r="U207" s="8"/>
     </row>
-    <row r="208" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A208" s="8" t="s">
         <v>21</v>
       </c>
@@ -14302,7 +14311,7 @@
       <c r="T208" s="8"/>
       <c r="U208" s="8"/>
     </row>
-    <row r="209" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:23" hidden="1">
       <c r="A209" s="8" t="s">
         <v>21</v>
       </c>
@@ -14353,7 +14362,7 @@
       <c r="V209" s="1"/>
       <c r="W209" s="1"/>
     </row>
-    <row r="210" spans="1:23" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:23" s="19" customFormat="1">
       <c r="A210" s="15" t="s">
         <v>21</v>
       </c>
@@ -14414,7 +14423,7 @@
       <c r="V210" s="21"/>
       <c r="W210" s="21"/>
     </row>
-    <row r="211" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:23" hidden="1">
       <c r="A211" s="8" t="s">
         <v>21</v>
       </c>
@@ -14465,7 +14474,7 @@
       <c r="V211" s="1"/>
       <c r="W211" s="1"/>
     </row>
-    <row r="212" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:23" hidden="1">
       <c r="A212" s="8" t="s">
         <v>21</v>
       </c>
@@ -14516,7 +14525,7 @@
       <c r="V212" s="1"/>
       <c r="W212" s="1"/>
     </row>
-    <row r="213" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:23" hidden="1">
       <c r="A213" s="8" t="s">
         <v>21</v>
       </c>
@@ -14569,7 +14578,7 @@
       <c r="V213" s="1"/>
       <c r="W213" s="1"/>
     </row>
-    <row r="214" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:23" hidden="1">
       <c r="A214" s="8" t="s">
         <v>21</v>
       </c>
@@ -14620,7 +14629,7 @@
       <c r="V214" s="1"/>
       <c r="W214" s="1"/>
     </row>
-    <row r="215" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:23" hidden="1">
       <c r="A215" s="8" t="s">
         <v>21</v>
       </c>
@@ -14669,7 +14678,7 @@
       <c r="V215" s="1"/>
       <c r="W215" s="1"/>
     </row>
-    <row r="216" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:23" hidden="1">
       <c r="A216" s="8" t="s">
         <v>21</v>
       </c>
@@ -14720,7 +14729,7 @@
       <c r="V216" s="1"/>
       <c r="W216" s="1"/>
     </row>
-    <row r="217" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:23" hidden="1">
       <c r="A217" s="8" t="s">
         <v>21</v>
       </c>
@@ -14773,7 +14782,7 @@
       <c r="V217" s="1"/>
       <c r="W217" s="1"/>
     </row>
-    <row r="218" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:23" hidden="1">
       <c r="A218" s="8" t="s">
         <v>21</v>
       </c>
@@ -14824,7 +14833,7 @@
       <c r="V218" s="1"/>
       <c r="W218" s="1"/>
     </row>
-    <row r="219" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:23" hidden="1">
       <c r="A219" s="8" t="s">
         <v>21</v>
       </c>
@@ -14875,7 +14884,7 @@
       <c r="V219" s="1"/>
       <c r="W219" s="1"/>
     </row>
-    <row r="220" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:23" hidden="1">
       <c r="A220" s="8" t="s">
         <v>21</v>
       </c>
@@ -14926,7 +14935,7 @@
       <c r="V220" s="1"/>
       <c r="W220" s="1"/>
     </row>
-    <row r="221" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:23" hidden="1">
       <c r="A221" s="8" t="s">
         <v>21</v>
       </c>
@@ -14977,7 +14986,7 @@
       <c r="V221" s="1"/>
       <c r="W221" s="1"/>
     </row>
-    <row r="222" spans="1:23" s="19" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:23" s="19" customFormat="1" ht="15">
       <c r="A222" s="15" t="s">
         <v>21</v>
       </c>
@@ -15038,7 +15047,7 @@
       <c r="V222" s="21"/>
       <c r="W222" s="21"/>
     </row>
-    <row r="223" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:23" hidden="1">
       <c r="A223" s="8" t="s">
         <v>21</v>
       </c>
@@ -15089,7 +15098,7 @@
       <c r="V223" s="1"/>
       <c r="W223" s="1"/>
     </row>
-    <row r="224" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:23" hidden="1">
       <c r="A224" s="8" t="s">
         <v>21</v>
       </c>
@@ -15140,7 +15149,7 @@
       <c r="V224" s="1"/>
       <c r="W224" s="1"/>
     </row>
-    <row r="225" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A225" s="8" t="s">
         <v>21</v>
       </c>
@@ -15189,7 +15198,7 @@
       <c r="T225" s="8"/>
       <c r="U225" s="8"/>
     </row>
-    <row r="226" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A226" s="8" t="s">
         <v>21</v>
       </c>
@@ -15236,7 +15245,7 @@
       <c r="T226" s="8"/>
       <c r="U226" s="8"/>
     </row>
-    <row r="227" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A227" s="8" t="s">
         <v>21</v>
       </c>
@@ -15285,7 +15294,7 @@
       <c r="T227" s="8"/>
       <c r="U227" s="8"/>
     </row>
-    <row r="228" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A228" s="8" t="s">
         <v>21</v>
       </c>
@@ -15334,7 +15343,7 @@
       <c r="T228" s="8"/>
       <c r="U228" s="8"/>
     </row>
-    <row r="229" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A229" s="8" t="s">
         <v>21</v>
       </c>
@@ -15383,7 +15392,7 @@
       <c r="T229" s="8"/>
       <c r="U229" s="8"/>
     </row>
-    <row r="230" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A230" s="8" t="s">
         <v>21</v>
       </c>
@@ -15432,7 +15441,7 @@
       <c r="T230" s="8"/>
       <c r="U230" s="8"/>
     </row>
-    <row r="231" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A231" s="8" t="s">
         <v>21</v>
       </c>
@@ -15481,7 +15490,7 @@
       <c r="T231" s="8"/>
       <c r="U231" s="8"/>
     </row>
-    <row r="232" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A232" s="8" t="s">
         <v>21</v>
       </c>
@@ -15528,7 +15537,7 @@
       <c r="T232" s="8"/>
       <c r="U232" s="8"/>
     </row>
-    <row r="233" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A233" s="8" t="s">
         <v>21</v>
       </c>
@@ -15577,7 +15586,7 @@
       <c r="T233" s="8"/>
       <c r="U233" s="8"/>
     </row>
-    <row r="234" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A234" s="8" t="s">
         <v>21</v>
       </c>
@@ -15626,7 +15635,7 @@
       <c r="T234" s="8"/>
       <c r="U234" s="8"/>
     </row>
-    <row r="235" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A235" s="8" t="s">
         <v>21</v>
       </c>
@@ -15677,7 +15686,7 @@
       <c r="T235" s="8"/>
       <c r="U235" s="8"/>
     </row>
-    <row r="236" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A236" s="8" t="s">
         <v>21</v>
       </c>
@@ -15726,7 +15735,7 @@
       <c r="T236" s="8"/>
       <c r="U236" s="8"/>
     </row>
-    <row r="237" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A237" s="8" t="s">
         <v>21</v>
       </c>
@@ -15775,7 +15784,7 @@
       <c r="T237" s="8"/>
       <c r="U237" s="8"/>
     </row>
-    <row r="238" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A238" s="8" t="s">
         <v>21</v>
       </c>
@@ -15824,7 +15833,7 @@
       <c r="T238" s="8"/>
       <c r="U238" s="8"/>
     </row>
-    <row r="239" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A239" s="8" t="s">
         <v>21</v>
       </c>
@@ -15873,7 +15882,7 @@
       <c r="T239" s="8"/>
       <c r="U239" s="8"/>
     </row>
-    <row r="240" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A240" s="8" t="s">
         <v>21</v>
       </c>
@@ -15924,7 +15933,7 @@
       <c r="T240" s="8"/>
       <c r="U240" s="8"/>
     </row>
-    <row r="241" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:23" hidden="1">
       <c r="A241" s="8" t="s">
         <v>21</v>
       </c>
@@ -15975,7 +15984,7 @@
       <c r="V241" s="1"/>
       <c r="W241" s="1"/>
     </row>
-    <row r="242" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:23" hidden="1">
       <c r="A242" s="8" t="s">
         <v>21</v>
       </c>
@@ -16026,7 +16035,7 @@
       <c r="V242" s="1"/>
       <c r="W242" s="1"/>
     </row>
-    <row r="243" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:23" hidden="1">
       <c r="A243" s="8" t="s">
         <v>21</v>
       </c>
@@ -16077,7 +16086,7 @@
       <c r="V243" s="1"/>
       <c r="W243" s="1"/>
     </row>
-    <row r="244" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:23" hidden="1">
       <c r="A244" s="8" t="s">
         <v>21</v>
       </c>
@@ -16128,7 +16137,7 @@
       <c r="V244" s="1"/>
       <c r="W244" s="1"/>
     </row>
-    <row r="245" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:23" hidden="1">
       <c r="A245" s="8" t="s">
         <v>21</v>
       </c>
@@ -16179,7 +16188,7 @@
       <c r="V245" s="1"/>
       <c r="W245" s="1"/>
     </row>
-    <row r="246" spans="1:23" s="19" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:23" s="19" customFormat="1" ht="15">
       <c r="A246" s="15" t="s">
         <v>21</v>
       </c>
@@ -16240,7 +16249,7 @@
       <c r="V246" s="21"/>
       <c r="W246" s="21"/>
     </row>
-    <row r="247" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:23" hidden="1">
       <c r="A247" s="8" t="s">
         <v>21</v>
       </c>
@@ -16291,7 +16300,7 @@
       <c r="V247" s="1"/>
       <c r="W247" s="1"/>
     </row>
-    <row r="248" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:23" hidden="1">
       <c r="A248" s="8" t="s">
         <v>21</v>
       </c>
@@ -16342,7 +16351,7 @@
       <c r="V248" s="1"/>
       <c r="W248" s="1"/>
     </row>
-    <row r="249" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:23" hidden="1">
       <c r="A249" s="8" t="s">
         <v>21</v>
       </c>
@@ -16393,7 +16402,7 @@
       <c r="V249" s="1"/>
       <c r="W249" s="1"/>
     </row>
-    <row r="250" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:23" hidden="1">
       <c r="A250" s="8" t="s">
         <v>21</v>
       </c>
@@ -16444,7 +16453,7 @@
       <c r="V250" s="1"/>
       <c r="W250" s="1"/>
     </row>
-    <row r="251" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:23" hidden="1">
       <c r="A251" s="8" t="s">
         <v>21</v>
       </c>
@@ -16495,7 +16504,7 @@
       <c r="V251" s="1"/>
       <c r="W251" s="1"/>
     </row>
-    <row r="252" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:23" hidden="1">
       <c r="A252" s="8" t="s">
         <v>21</v>
       </c>
@@ -16546,7 +16555,7 @@
       <c r="V252" s="1"/>
       <c r="W252" s="1"/>
     </row>
-    <row r="253" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:23" hidden="1">
       <c r="A253" s="8" t="s">
         <v>21</v>
       </c>
@@ -16597,7 +16606,7 @@
       <c r="V253" s="1"/>
       <c r="W253" s="1"/>
     </row>
-    <row r="254" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:23" hidden="1">
       <c r="A254" s="8" t="s">
         <v>21</v>
       </c>
@@ -16648,7 +16657,7 @@
       <c r="V254" s="1"/>
       <c r="W254" s="1"/>
     </row>
-    <row r="255" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:23" hidden="1">
       <c r="A255" s="8" t="s">
         <v>21</v>
       </c>
@@ -16699,7 +16708,7 @@
       <c r="V255" s="1"/>
       <c r="W255" s="1"/>
     </row>
-    <row r="256" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:23" hidden="1">
       <c r="A256" s="8" t="s">
         <v>21</v>
       </c>
@@ -16750,7 +16759,7 @@
       <c r="V256" s="1"/>
       <c r="W256" s="1"/>
     </row>
-    <row r="257" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:23" hidden="1">
       <c r="A257" s="8" t="s">
         <v>21</v>
       </c>
@@ -16801,7 +16810,7 @@
       <c r="V257" s="1"/>
       <c r="W257" s="1"/>
     </row>
-    <row r="258" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:23" hidden="1">
       <c r="A258" s="8" t="s">
         <v>21</v>
       </c>
@@ -16852,7 +16861,7 @@
       <c r="V258" s="1"/>
       <c r="W258" s="1"/>
     </row>
-    <row r="259" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:23" hidden="1">
       <c r="A259" s="8" t="s">
         <v>21</v>
       </c>
@@ -16903,7 +16912,7 @@
       <c r="V259" s="1"/>
       <c r="W259" s="1"/>
     </row>
-    <row r="260" spans="1:23" ht="22" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:23" ht="23.25">
       <c r="A260" s="8" t="s">
         <v>21</v>
       </c>
@@ -16968,7 +16977,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="261" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:23" hidden="1">
       <c r="A261" s="8" t="s">
         <v>21</v>
       </c>
@@ -17019,7 +17028,7 @@
       <c r="V261" s="1"/>
       <c r="W261" s="1"/>
     </row>
-    <row r="262" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:23" hidden="1">
       <c r="A262" s="8" t="s">
         <v>21</v>
       </c>
@@ -17072,7 +17081,7 @@
       <c r="V262" s="1"/>
       <c r="W262" s="1"/>
     </row>
-    <row r="263" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:23" hidden="1">
       <c r="A263" s="8" t="s">
         <v>21</v>
       </c>
@@ -17123,7 +17132,7 @@
       <c r="V263" s="1"/>
       <c r="W263" s="1"/>
     </row>
-    <row r="264" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:23" hidden="1">
       <c r="A264" s="8" t="s">
         <v>21</v>
       </c>
@@ -17172,7 +17181,7 @@
       <c r="V264" s="1"/>
       <c r="W264" s="1"/>
     </row>
-    <row r="265" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:23" hidden="1">
       <c r="A265" s="8" t="s">
         <v>21</v>
       </c>
@@ -17225,7 +17234,7 @@
       <c r="V265" s="1"/>
       <c r="W265" s="1"/>
     </row>
-    <row r="266" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:23" hidden="1">
       <c r="A266" s="8" t="s">
         <v>21</v>
       </c>
@@ -17276,7 +17285,7 @@
       <c r="V266" s="1"/>
       <c r="W266" s="1"/>
     </row>
-    <row r="267" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:23" hidden="1">
       <c r="A267" s="8" t="s">
         <v>21</v>
       </c>
@@ -17327,7 +17336,7 @@
       <c r="V267" s="1"/>
       <c r="W267" s="1"/>
     </row>
-    <row r="268" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:23" hidden="1">
       <c r="A268" s="8" t="s">
         <v>21</v>
       </c>
@@ -17378,7 +17387,7 @@
       <c r="V268" s="1"/>
       <c r="W268" s="1"/>
     </row>
-    <row r="269" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:23" hidden="1">
       <c r="A269" s="8" t="s">
         <v>21</v>
       </c>
@@ -17431,7 +17440,7 @@
       <c r="V269" s="1"/>
       <c r="W269" s="1"/>
     </row>
-    <row r="270" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:23" hidden="1">
       <c r="A270" s="8" t="s">
         <v>21</v>
       </c>
@@ -17482,7 +17491,7 @@
       <c r="V270" s="1"/>
       <c r="W270" s="1"/>
     </row>
-    <row r="271" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:23" hidden="1">
       <c r="A271" s="8" t="s">
         <v>21</v>
       </c>
@@ -17533,7 +17542,7 @@
       <c r="V271" s="1"/>
       <c r="W271" s="1"/>
     </row>
-    <row r="272" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:23" hidden="1">
       <c r="A272" s="8" t="s">
         <v>21</v>
       </c>
@@ -17584,7 +17593,7 @@
       <c r="V272" s="1"/>
       <c r="W272" s="1"/>
     </row>
-    <row r="273" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A273" s="8" t="s">
         <v>21</v>
       </c>
@@ -17633,7 +17642,7 @@
       <c r="T273" s="8"/>
       <c r="U273" s="8"/>
     </row>
-    <row r="274" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A274" s="8" t="s">
         <v>21</v>
       </c>
@@ -17682,7 +17691,7 @@
       <c r="T274" s="8"/>
       <c r="U274" s="8"/>
     </row>
-    <row r="275" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A275" s="8" t="s">
         <v>21</v>
       </c>
@@ -17731,7 +17740,7 @@
       <c r="T275" s="8"/>
       <c r="U275" s="8"/>
     </row>
-    <row r="276" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A276" s="8" t="s">
         <v>21</v>
       </c>
@@ -17780,7 +17789,7 @@
       <c r="T276" s="8"/>
       <c r="U276" s="8"/>
     </row>
-    <row r="277" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A277" s="8" t="s">
         <v>21</v>
       </c>
@@ -17829,7 +17838,7 @@
       <c r="T277" s="8"/>
       <c r="U277" s="8"/>
     </row>
-    <row r="278" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A278" s="8" t="s">
         <v>21</v>
       </c>
@@ -17878,7 +17887,7 @@
       <c r="T278" s="8"/>
       <c r="U278" s="8"/>
     </row>
-    <row r="279" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A279" s="8" t="s">
         <v>21</v>
       </c>
@@ -17927,7 +17936,7 @@
       <c r="T279" s="8"/>
       <c r="U279" s="8"/>
     </row>
-    <row r="280" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A280" s="8" t="s">
         <v>21</v>
       </c>
@@ -17976,7 +17985,7 @@
       <c r="T280" s="8"/>
       <c r="U280" s="8"/>
     </row>
-    <row r="281" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A281" s="8" t="s">
         <v>21</v>
       </c>
@@ -18025,7 +18034,7 @@
       <c r="T281" s="8"/>
       <c r="U281" s="8"/>
     </row>
-    <row r="282" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A282" s="8" t="s">
         <v>21</v>
       </c>
@@ -18074,7 +18083,7 @@
       <c r="T282" s="8"/>
       <c r="U282" s="8"/>
     </row>
-    <row r="283" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A283" s="8" t="s">
         <v>21</v>
       </c>
@@ -18123,7 +18132,7 @@
       <c r="T283" s="8"/>
       <c r="U283" s="8"/>
     </row>
-    <row r="284" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A284" s="8" t="s">
         <v>21</v>
       </c>
@@ -18172,7 +18181,7 @@
       <c r="T284" s="8"/>
       <c r="U284" s="8"/>
     </row>
-    <row r="285" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A285" s="8" t="s">
         <v>21</v>
       </c>
@@ -18221,7 +18230,7 @@
       <c r="T285" s="8"/>
       <c r="U285" s="8"/>
     </row>
-    <row r="286" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A286" s="8" t="s">
         <v>21</v>
       </c>
@@ -18272,7 +18281,7 @@
       <c r="T286" s="8"/>
       <c r="U286" s="8"/>
     </row>
-    <row r="287" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A287" s="8" t="s">
         <v>21</v>
       </c>
@@ -18321,7 +18330,7 @@
       <c r="T287" s="8"/>
       <c r="U287" s="8"/>
     </row>
-    <row r="288" spans="1:21" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:21" s="1" customFormat="1" hidden="1">
       <c r="A288" s="8" t="s">
         <v>21</v>
       </c>
@@ -18370,7 +18379,7 @@
       <c r="T288" s="8"/>
       <c r="U288" s="8"/>
     </row>
-    <row r="289" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:23" hidden="1">
       <c r="A289" s="8" t="s">
         <v>21</v>
       </c>
@@ -18421,7 +18430,7 @@
       <c r="V289" s="1"/>
       <c r="W289" s="1"/>
     </row>
-    <row r="290" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:23" hidden="1">
       <c r="A290" s="8" t="s">
         <v>21</v>
       </c>
@@ -18472,7 +18481,7 @@
       <c r="V290" s="1"/>
       <c r="W290" s="1"/>
     </row>
-    <row r="291" spans="1:23" s="19" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:23" s="19" customFormat="1" ht="15">
       <c r="A291" s="15" t="s">
         <v>21</v>
       </c>
@@ -18533,7 +18542,7 @@
       <c r="V291" s="21"/>
       <c r="W291" s="21"/>
     </row>
-    <row r="292" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:23" hidden="1">
       <c r="A292" s="8" t="s">
         <v>21</v>
       </c>
@@ -18584,7 +18593,7 @@
       <c r="V292" s="1"/>
       <c r="W292" s="1"/>
     </row>
-    <row r="293" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:23" hidden="1">
       <c r="A293" s="8" t="s">
         <v>21</v>
       </c>
@@ -18637,7 +18646,7 @@
       <c r="V293" s="1"/>
       <c r="W293" s="1"/>
     </row>
-    <row r="294" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:23" hidden="1">
       <c r="A294" s="8" t="s">
         <v>21</v>
       </c>
@@ -18690,7 +18699,7 @@
       <c r="V294" s="1"/>
       <c r="W294" s="1"/>
     </row>
-    <row r="295" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:23" hidden="1">
       <c r="A295" s="8" t="s">
         <v>21</v>
       </c>
@@ -18742,7 +18751,7 @@
       <c r="W295" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U295" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:U295">
     <filterColumn colId="6">
       <filters>
         <filter val="Paruchuru Praveena Kumari (prparuch)"/>
@@ -18750,26 +18759,26 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="L56" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L59" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="L62" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="L64" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="L77" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="L86" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="L97" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="L102" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="L125" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="L130" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="L143" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="L147" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="L222" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="L260" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="L246" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="L291" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="L74" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="L107" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="L124" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="L146" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="L56" r:id="rId1"/>
+    <hyperlink ref="L59" r:id="rId2"/>
+    <hyperlink ref="L62" r:id="rId3"/>
+    <hyperlink ref="L64" r:id="rId4"/>
+    <hyperlink ref="L77" r:id="rId5"/>
+    <hyperlink ref="L86" r:id="rId6"/>
+    <hyperlink ref="L97" r:id="rId7"/>
+    <hyperlink ref="L102" r:id="rId8"/>
+    <hyperlink ref="L125" r:id="rId9"/>
+    <hyperlink ref="L130" r:id="rId10"/>
+    <hyperlink ref="L143" r:id="rId11"/>
+    <hyperlink ref="L147" r:id="rId12"/>
+    <hyperlink ref="L222" r:id="rId13"/>
+    <hyperlink ref="L260" r:id="rId14"/>
+    <hyperlink ref="L246" r:id="rId15"/>
+    <hyperlink ref="L291" r:id="rId16"/>
+    <hyperlink ref="L74" r:id="rId17"/>
+    <hyperlink ref="L107" r:id="rId18"/>
+    <hyperlink ref="L124" r:id="rId19"/>
+    <hyperlink ref="L146" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId21"/>

</xml_diff>